<commit_message>
more formulas testing vs. in-excel
</commit_message>
<xml_diff>
--- a/Car Price List.xlsx
+++ b/Car Price List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itzdu\Desktop\Database Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A79DA26-3263-4005-88B0-AEB0F347E610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC75E57D-2353-4CEE-909B-90C001D071FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="492" windowWidth="30936" windowHeight="16896" xr2:uid="{5DF00017-B3B6-45A6-B9B7-DF4726A0B877}"/>
   </bookViews>
@@ -705,9 +705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3025D9-5964-4081-B1C3-FA8B7471B24E}">
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>